<commit_message>
Fixed footprints for sharing
</commit_message>
<xml_diff>
--- a/PCB/JAARK_PCB_MOTOR/JAARK_PCB_MOTOR.xlsx
+++ b/PCB/JAARK_PCB_MOTOR/JAARK_PCB_MOTOR.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty" localSheetId="0">'JAARK_PCB_MOTOR'!$G$1</definedName>
-    <definedName name="PURCHASE_DESCRIPTION" localSheetId="0">'JAARK_PCB_MOTOR'!$G$28</definedName>
+    <definedName name="PURCHASE_DESCRIPTION" localSheetId="0">'JAARK_PCB_MOTOR'!$G$29</definedName>
     <definedName name="TotalCost" localSheetId="0">'JAARK_PCB_MOTOR'!$G$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -503,6 +503,41 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
+     1   $7.18      $7.18
+    10   $5.54     $55.41
+    25   $5.13    $128.28
+   100   $4.68    $468.01
+   250   $4.47  $1,116.27
+   500   $4.34  $2,167.75</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Desc: IC FULL BRIDGE DRIVER 20SOIC
+Footprint: 20-SOIC (0.295", 7.50mm Width)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
      1   $0.86      $0.86
     10   $0.62      $6.24
     25   $0.54     $13.59
@@ -511,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M14" authorId="0">
+    <comment ref="M15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -524,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0">
+    <comment ref="H16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -537,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0">
+    <comment ref="J16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -556,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M15" authorId="0">
+    <comment ref="M16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0">
+    <comment ref="J17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -589,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M16" authorId="0">
+    <comment ref="M17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -606,7 +641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0">
+    <comment ref="J18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -626,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M17" authorId="0">
+    <comment ref="M18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -640,7 +675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0">
+    <comment ref="J19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -658,7 +693,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M18" authorId="0">
+    <comment ref="M19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -671,7 +706,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0">
+    <comment ref="J20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -691,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M19" authorId="0">
+    <comment ref="M20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -705,7 +740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0">
+    <comment ref="J21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -728,7 +763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M20" authorId="0">
+    <comment ref="M21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -747,7 +782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0">
+    <comment ref="J22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M21" authorId="0">
+    <comment ref="M22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -786,7 +821,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0">
+    <comment ref="J23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -809,7 +844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0">
+    <comment ref="M23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -828,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="0">
+    <comment ref="J24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -847,7 +882,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M23" authorId="0">
+    <comment ref="M24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -866,7 +901,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0">
+    <comment ref="J25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M24" authorId="0">
+    <comment ref="M25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -905,7 +940,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0">
+    <comment ref="J26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -925,7 +960,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M25" authorId="0">
+    <comment ref="M26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -944,7 +979,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0">
+    <comment ref="F28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -957,7 +992,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="0">
+    <comment ref="I28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -970,7 +1005,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0">
+    <comment ref="F29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -988,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -1053,13 +1088,19 @@
     <t>TPS564242DRLR</t>
   </si>
   <si>
-    <t>IC2,IC3</t>
+    <t>IC2,IC3,IC5-IC8</t>
   </si>
   <si>
     <t>PJA3404_R1_00001</t>
   </si>
   <si>
-    <t>J1,J4</t>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>HIP4080AIBZT</t>
+  </si>
+  <si>
+    <t>J1,J3,J4</t>
   </si>
   <si>
     <t>1984617</t>
@@ -1173,6 +1214,9 @@
     <t>3757-PJA3404_R1_00001CT-ND</t>
   </si>
   <si>
+    <t>HIP4080AIBZTCT-ND</t>
+  </si>
+  <si>
     <t>277-1721-ND</t>
   </si>
   <si>
@@ -1233,7 +1277,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>2026-02-03 20:28:56 (file)</t>
+    <t>2026-02-04 07:59:11 (file)</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1248,7 +1292,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2026-02-03 20:29:17</t>
+    <t>2026-02-04 08:04:06</t>
   </si>
   <si>
     <t>KiCost® v1.1.20</t>
@@ -1761,7 +1805,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
@@ -1789,13 +1833,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G1" s="3">
         <v>1</v>
@@ -1803,46 +1847,46 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>14.732</v>
+        <v>23.892</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G3" s="5">
-        <f>SUM(G7:G25)</f>
-        <v>14.732</v>
+        <f>SUM(G7:G26)</f>
+        <v>23.892</v>
       </c>
       <c r="L3" s="5">
-        <f>SUM(L7:L25)</f>
-        <v>14.732</v>
+        <f>SUM(L7:L26)</f>
+        <v>23.892</v>
       </c>
       <c r="M3" s="6" t="str">
-        <f>(COUNTA(L7:L25)&amp;" of "&amp;ROWS(L7:L25)&amp;" parts found")</f>
-        <v>19 of 19 parts found</v>
+        <f>(COUNTA(L7:L26)&amp;" of "&amp;ROWS(L7:L26)&amp;" parts found")</f>
+        <v>20 of 20 parts found</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1856,7 +1900,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -1887,22 +1931,22 @@
         <v>7</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1946,7 +1990,7 @@
         <v>0.32</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1990,7 +2034,7 @@
         <v>0.15</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2034,7 +2078,7 @@
         <v>0.08</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2078,7 +2122,7 @@
         <v>1.13</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
@@ -2122,7 +2166,7 @@
         <v>0.112</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2166,7 +2210,7 @@
         <v>0.56</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2183,8 +2227,8 @@
         <v>22</v>
       </c>
       <c r="E13" s="10">
-        <f>CEILING(BoardQty*2.0,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6.0,1)</f>
+        <v>6</v>
       </c>
       <c r="F13" s="11">
         <f>IF(MIN(J13)&lt;&gt;0,MIN(J13),"")</f>
@@ -2192,7 +2236,7 @@
       </c>
       <c r="G13" s="12">
         <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
-        <v>0.56</v>
+        <v>1.68</v>
       </c>
       <c r="H13" s="10">
         <v>52634</v>
@@ -2207,10 +2251,10 @@
       </c>
       <c r="L13" s="12">
         <f>IFERROR(IF(I13="",E13,I13)*J13,"")</f>
-        <v>0.56</v>
+        <v>1.68</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2227,34 +2271,34 @@
         <v>24</v>
       </c>
       <c r="E14" s="10">
-        <f>CEILING(BoardQty*2.0,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*1.0,1)</f>
+        <v>1</v>
       </c>
       <c r="F14" s="11">
         <f>IF(MIN(J14)&lt;&gt;0,MIN(J14),"")</f>
-        <v>0.86</v>
+        <v>7.18</v>
       </c>
       <c r="G14" s="12">
         <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
-        <v>1.72</v>
+        <v>7.18</v>
       </c>
       <c r="H14" s="10">
-        <v>12408</v>
+        <v>8140</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="11">
-        <f>IFERROR(IF(OR(I14&gt;=K14,E14&gt;=K14),LOOKUP(IF(I14="",E14,I14),{0,1,10,25,50,100},{0.0,0.86,0.624,0.5436,0.5164,0.4631}),"MOQ="&amp;K14),"")</f>
-        <v>0.86</v>
+        <f>IFERROR(IF(OR(I14&gt;=K14,E14&gt;=K14),LOOKUP(IF(I14="",E14,I14),{0,1,10,25,100,250,500},{0.0,7.18,5.541,5.1312,4.6801,4.46508,4.3355}),"MOQ="&amp;K14),"")</f>
+        <v>7.18</v>
       </c>
       <c r="K14" s="10">
         <v>1</v>
       </c>
       <c r="L14" s="12">
         <f>IFERROR(IF(I14="",E14,I14)*J14,"")</f>
-        <v>1.72</v>
+        <v>7.18</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2271,34 +2315,34 @@
         <v>26</v>
       </c>
       <c r="E15" s="10">
-        <f>CEILING(BoardQty*1.0,1)</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3.0,1)</f>
+        <v>3</v>
       </c>
       <c r="F15" s="11">
         <f>IF(MIN(J15)&lt;&gt;0,MIN(J15),"")</f>
-        <v>3.57</v>
+        <v>0.86</v>
       </c>
       <c r="G15" s="12">
         <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
-        <v>3.57</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>63</v>
+        <v>2.58</v>
+      </c>
+      <c r="H15" s="10">
+        <v>12408</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="11">
-        <f>IFERROR(IF(OR(I15&gt;=K15,E15&gt;=K15),LOOKUP(IF(I15="",E15,I15),{0,1,10,100,500},{0.0,3.57,3.031,2.5761,2.38658}),"MOQ="&amp;K15),"")</f>
-        <v>3.57</v>
+        <f>IFERROR(IF(OR(I15&gt;=K15,E15&gt;=K15),LOOKUP(IF(I15="",E15,I15),{0,1,10,25,50,100},{0.0,0.86,0.624,0.5436,0.5164,0.4631}),"MOQ="&amp;K15),"")</f>
+        <v>0.86</v>
       </c>
       <c r="K15" s="10">
         <v>1</v>
       </c>
       <c r="L15" s="12">
         <f>IFERROR(IF(I15="",E15,I15)*J15,"")</f>
-        <v>3.57</v>
+        <v>2.58</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2320,29 +2364,29 @@
       </c>
       <c r="F16" s="11">
         <f>IF(MIN(J16)&lt;&gt;0,MIN(J16),"")</f>
-        <v>1.94</v>
+        <v>3.57</v>
       </c>
       <c r="G16" s="12">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
-        <v>1.94</v>
-      </c>
-      <c r="H16" s="10">
-        <v>1841</v>
+        <v>3.57</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="11">
-        <f>IFERROR(IF(OR(I16&gt;=K16,E16&gt;=K16),LOOKUP(IF(I16="",E16,I16),{0,1,10,50,100,500},{0.0,1.94,1.898,1.815,1.672,1.541}),"MOQ="&amp;K16),"")</f>
-        <v>1.94</v>
+        <f>IFERROR(IF(OR(I16&gt;=K16,E16&gt;=K16),LOOKUP(IF(I16="",E16,I16),{0,1,10,100,500},{0.0,3.57,3.031,2.5761,2.38658}),"MOQ="&amp;K16),"")</f>
+        <v>3.57</v>
       </c>
       <c r="K16" s="10">
         <v>1</v>
       </c>
       <c r="L16" s="12">
         <f>IFERROR(IF(I16="",E16,I16)*J16,"")</f>
-        <v>1.94</v>
+        <v>3.57</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2350,57 +2394,57 @@
         <v>29</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E17" s="10">
-        <f>CEILING(BoardQty*3.0,1)</f>
-        <v>3</v>
+        <f>CEILING(BoardQty*1.0,1)</f>
+        <v>1</v>
       </c>
       <c r="F17" s="11">
         <f>IF(MIN(J17)&lt;&gt;0,MIN(J17),"")</f>
-        <v>0.37</v>
+        <v>1.94</v>
       </c>
       <c r="G17" s="12">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
-        <v>1.11</v>
+        <v>1.94</v>
       </c>
       <c r="H17" s="10">
-        <v>47397</v>
+        <v>1841</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="11">
-        <f>IFERROR(IF(OR(I17&gt;=K17,E17&gt;=K17),LOOKUP(IF(I17="",E17,I17),{0,1,10,100,500,1000},{0.0,0.37,0.228,0.143,0.10622,0.09431}),"MOQ="&amp;K17),"")</f>
-        <v>0.37</v>
+        <f>IFERROR(IF(OR(I17&gt;=K17,E17&gt;=K17),LOOKUP(IF(I17="",E17,I17),{0,1,10,50,100,500},{0.0,1.94,1.898,1.815,1.672,1.541}),"MOQ="&amp;K17),"")</f>
+        <v>1.94</v>
       </c>
       <c r="K17" s="10">
         <v>1</v>
       </c>
       <c r="L17" s="12">
         <f>IFERROR(IF(I17="",E17,I17)*J17,"")</f>
-        <v>1.11</v>
+        <v>1.94</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="E18" s="10">
         <f>CEILING(BoardQty*3.0,1)</f>
@@ -2408,37 +2452,37 @@
       </c>
       <c r="F18" s="11">
         <f>IF(MIN(J18)&lt;&gt;0,MIN(J18),"")</f>
-        <v/>
+        <v>0.37</v>
       </c>
       <c r="G18" s="12">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
-        <v/>
+        <v>1.11</v>
       </c>
       <c r="H18" s="10">
-        <v>12000</v>
+        <v>47397</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="11">
-        <f>IFERROR(IF(OR(I18&gt;=K18,E18&gt;=K18),LOOKUP(IF(I18="",E18,I18),{0,1,6000,12000,18000},{0.0,0.5734,0.5734,0.54606,0.53265}),"MOQ="&amp;K18),"")</f>
-        <v/>
+        <f>IFERROR(IF(OR(I18&gt;=K18,E18&gt;=K18),LOOKUP(IF(I18="",E18,I18),{0,1,10,100,500,1000},{0.0,0.37,0.228,0.143,0.10622,0.09431}),"MOQ="&amp;K18),"")</f>
+        <v>0.37</v>
       </c>
       <c r="K18" s="10">
-        <v>6000</v>
+        <v>1</v>
       </c>
       <c r="L18" s="12">
         <f>IFERROR(IF(I18="",E18,I18)*J18,"")</f>
-        <v/>
+        <v>1.11</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>9</v>
@@ -2447,34 +2491,34 @@
         <v>36</v>
       </c>
       <c r="E19" s="10">
-        <f>CEILING(BoardQty*4.0,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*3.0,1)</f>
+        <v>3</v>
       </c>
       <c r="F19" s="11">
         <f>IF(MIN(J19)&lt;&gt;0,MIN(J19),"")</f>
-        <v>0.62</v>
+        <v/>
       </c>
       <c r="G19" s="12">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
-        <v>2.48</v>
+        <v/>
       </c>
       <c r="H19" s="10">
-        <v>63265</v>
+        <v>12000</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="11">
-        <f>IFERROR(IF(OR(I19&gt;=K19,E19&gt;=K19),LOOKUP(IF(I19="",E19,I19),{0,1,10,100,500,1000},{0.0,0.62,0.381,0.2433,0.18394,0.16479}),"MOQ="&amp;K19),"")</f>
-        <v>0.62</v>
+        <f>IFERROR(IF(OR(I19&gt;=K19,E19&gt;=K19),LOOKUP(IF(I19="",E19,I19),{0,1,6000,12000,18000},{0.0,0.5734,0.5734,0.54606,0.53265}),"MOQ="&amp;K19),"")</f>
+        <v/>
       </c>
       <c r="K19" s="10">
-        <v>1</v>
+        <v>6000</v>
       </c>
       <c r="L19" s="12">
         <f>IFERROR(IF(I19="",E19,I19)*J19,"")</f>
-        <v>2.48</v>
+        <v/>
       </c>
       <c r="M19" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -2491,34 +2535,34 @@
         <v>38</v>
       </c>
       <c r="E20" s="10">
-        <f>CEILING(BoardQty*1.0,1)</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4.0,1)</f>
+        <v>4</v>
       </c>
       <c r="F20" s="11">
         <f>IF(MIN(J20)&lt;&gt;0,MIN(J20),"")</f>
-        <v>0.1</v>
+        <v>0.62</v>
       </c>
       <c r="G20" s="12">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
-        <v>0.1</v>
+        <v>2.48</v>
       </c>
       <c r="H20" s="10">
-        <v>1227152</v>
+        <v>63265</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="11">
-        <f>IFERROR(IF(OR(I20&gt;=K20,E20&gt;=K20),LOOKUP(IF(I20="",E20,I20),{0,1,10,25,50,100,250,500,1000},{0.0,0.1,0.035,0.026,0.0214,0.0176,0.01392,0.0118,0.01014}),"MOQ="&amp;K20),"")</f>
-        <v>0.1</v>
+        <f>IFERROR(IF(OR(I20&gt;=K20,E20&gt;=K20),LOOKUP(IF(I20="",E20,I20),{0,1,10,100,500,1000},{0.0,0.62,0.381,0.2433,0.18394,0.16479}),"MOQ="&amp;K20),"")</f>
+        <v>0.62</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
       </c>
       <c r="L20" s="12">
         <f>IFERROR(IF(I20="",E20,I20)*J20,"")</f>
-        <v>0.1</v>
+        <v>2.48</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -2547,11 +2591,11 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="10">
-        <v>95107</v>
+        <v>1227152</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="11">
-        <f>IFERROR(IF(OR(I21&gt;=K21,E21&gt;=K21),LOOKUP(IF(I21="",E21,I21),{0,1,10,25,50,100},{0.0,0.1,0.011,0.0096,0.0082,0.0077}),"MOQ="&amp;K21),"")</f>
+        <f>IFERROR(IF(OR(I21&gt;=K21,E21&gt;=K21),LOOKUP(IF(I21="",E21,I21),{0,1,10,25,50,100,250,500,1000},{0.0,0.1,0.035,0.026,0.0214,0.0176,0.01392,0.0118,0.01014}),"MOQ="&amp;K21),"")</f>
         <v>0.1</v>
       </c>
       <c r="K21" s="10">
@@ -2562,7 +2606,7 @@
         <v>0.1</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2591,11 +2635,11 @@
         <v>0.1</v>
       </c>
       <c r="H22" s="10">
-        <v>130853</v>
+        <v>95107</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="11">
-        <f>IFERROR(IF(OR(I22&gt;=K22,E22&gt;=K22),LOOKUP(IF(I22="",E22,I22),{0,1,10,25,50,100,250,500,1000},{0.0,0.1,0.08,0.0744,0.0704,0.0664,0.06164,0.05832,0.0553}),"MOQ="&amp;K22),"")</f>
+        <f>IFERROR(IF(OR(I22&gt;=K22,E22&gt;=K22),LOOKUP(IF(I22="",E22,I22),{0,1,10,25,50,100},{0.0,0.1,0.011,0.0096,0.0082,0.0077}),"MOQ="&amp;K22),"")</f>
         <v>0.1</v>
       </c>
       <c r="K22" s="10">
@@ -2606,7 +2650,7 @@
         <v>0.1</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2635,11 +2679,11 @@
         <v>0.1</v>
       </c>
       <c r="H23" s="10">
-        <v>201092</v>
+        <v>130853</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11">
-        <f>IFERROR(IF(OR(I23&gt;=K23,E23&gt;=K23),LOOKUP(IF(I23="",E23,I23),{0,1,10,25,50},{0.0,0.1,0.01,0.0092,0.0082}),"MOQ="&amp;K23),"")</f>
+        <f>IFERROR(IF(OR(I23&gt;=K23,E23&gt;=K23),LOOKUP(IF(I23="",E23,I23),{0,1,10,25,50,100,250,500,1000},{0.0,0.1,0.08,0.0744,0.0704,0.0664,0.06164,0.05832,0.0553}),"MOQ="&amp;K23),"")</f>
         <v>0.1</v>
       </c>
       <c r="K23" s="10">
@@ -2650,7 +2694,7 @@
         <v>0.1</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2667,8 +2711,8 @@
         <v>46</v>
       </c>
       <c r="E24" s="10">
-        <f>CEILING(BoardQty*4.0,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*1.0,1)</f>
+        <v>1</v>
       </c>
       <c r="F24" s="11">
         <f>IF(MIN(J24)&lt;&gt;0,MIN(J24),"")</f>
@@ -2676,14 +2720,14 @@
       </c>
       <c r="G24" s="12">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H24" s="10">
-        <v>31486</v>
+        <v>201092</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="11">
-        <f>IFERROR(IF(OR(I24&gt;=K24,E24&gt;=K24),LOOKUP(IF(I24="",E24,I24),{0,1,10,25,50,100},{0.0,0.1,0.054,0.0512,0.0458,0.0078}),"MOQ="&amp;K24),"")</f>
+        <f>IFERROR(IF(OR(I24&gt;=K24,E24&gt;=K24),LOOKUP(IF(I24="",E24,I24),{0,1,10,25,50},{0.0,0.1,0.01,0.0092,0.0082}),"MOQ="&amp;K24),"")</f>
         <v>0.1</v>
       </c>
       <c r="K24" s="10">
@@ -2691,10 +2735,10 @@
       </c>
       <c r="L24" s="12">
         <f>IFERROR(IF(I24="",E24,I24)*J24,"")</f>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2711,8 +2755,8 @@
         <v>48</v>
       </c>
       <c r="E25" s="10">
-        <f>CEILING(BoardQty*2.0,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*4.0,1)</f>
+        <v>4</v>
       </c>
       <c r="F25" s="11">
         <f>IF(MIN(J25)&lt;&gt;0,MIN(J25),"")</f>
@@ -2720,14 +2764,14 @@
       </c>
       <c r="G25" s="12">
         <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H25" s="10">
-        <v>1225788</v>
+        <v>31486</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="11">
-        <f>IFERROR(IF(OR(I25&gt;=K25,E25&gt;=K25),LOOKUP(IF(I25="",E25,I25),{0,1,10,25,50,100},{0.0,0.1,0.009,0.0088,0.0082,0.0075}),"MOQ="&amp;K25),"")</f>
+        <f>IFERROR(IF(OR(I25&gt;=K25,E25&gt;=K25),LOOKUP(IF(I25="",E25,I25),{0,1,10,25,50,100},{0.0,0.1,0.054,0.0512,0.0458,0.0078}),"MOQ="&amp;K25),"")</f>
         <v>0.1</v>
       </c>
       <c r="K25" s="10">
@@ -2735,59 +2779,93 @@
       </c>
       <c r="L25" s="12">
         <f>IFERROR(IF(I25="",E25,I25)*J25,"")</f>
+        <v>0.4</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="10">
+        <f>CEILING(BoardQty*2.0,1)</f>
+        <v>2</v>
+      </c>
+      <c r="F26" s="11">
+        <f>IF(MIN(J26)&lt;&gt;0,MIN(J26),"")</f>
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="12">
+        <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
         <v>0.2</v>
       </c>
-      <c r="M25" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="F27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="5">
-        <f>SUM(L27)</f>
+      <c r="H26" s="10">
+        <v>1225788</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="11">
+        <f>IFERROR(IF(OR(I26&gt;=K26,E26&gt;=K26),LOOKUP(IF(I26="",E26,I26),{0,1,10,25,50,100},{0.0,0.1,0.009,0.0088,0.0082,0.0075}),"MOQ="&amp;K26),"")</f>
+        <v>0.1</v>
+      </c>
+      <c r="K26" s="10">
+        <v>1</v>
+      </c>
+      <c r="L26" s="12">
+        <f>IFERROR(IF(I26="",E26,I26)*J26,"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="F28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="5">
+        <f>SUM(L28)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="I27" s="6">
-        <f>IFERROR(IF(COUNTIF(I7:I25,"&gt;0")&gt;0,COUNTIF(I7:I25,"&gt;0")&amp;" of "&amp;(ROWS(K7:K25)-COUNTBLANK(K7:K25))&amp;" parts purchased",""),"")</f>
+      <c r="H28" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="6">
+        <f>IFERROR(IF(COUNTIF(I7:I26,"&gt;0")&gt;0,COUNTIF(I7:I26,"&gt;0")&amp;" of "&amp;(ROWS(K7:K26)-COUNTBLANK(K7:K26))&amp;" parts purchased",""),"")</f>
         <v/>
       </c>
-      <c r="L27" s="5">
-        <f>SUMIF(I7:I25,"&gt;0",L7:L25)</f>
+      <c r="L28" s="5">
+        <f>SUMIF(I7:I26,"&gt;0",L7:L26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="16">
-        <f>CONCATENATE(I48,I49,I50,I51,I52,I53,I54,I55,I56,I57,I58,I59,I60,I61,I62,I63,I64,I65,I66)</f>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="16">
+        <f>CONCATENATE(I50,I51,I52,I53,I54,I55,I56,I57,I58,I59,I60,I61,I62,I63,I64,I65,I66,I67,I68,I69)</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="9:9" ht="30" hidden="1" customHeight="1">
-      <c r="I48" t="str">
-        <f t="array" ref="I48:I66">IF(ISNUMBER(I7:I25)*(I7:I25&gt;=K7:K25)*(M7:M25&lt;&gt;""),TEXT(ROUNDUP(I7:I25/IF(ISNUMBER(K7:K25),K7:K25,1),0)*K7:K25,"##0")&amp;","&amp;M7:M25&amp;","&amp;SUBSTITUTE(SUBSTITUTE(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A25,",",";"),"
+    <row r="50" spans="9:9" ht="30" hidden="1" customHeight="1">
+      <c r="I50" t="str">
+        <f t="array" ref="I50:I69">IF(ISNUMBER(I7:I26)*(I7:I26&gt;=K7:K26)*(M7:M26&lt;&gt;""),TEXT(ROUNDUP(I7:I26/IF(ISNUMBER(K7:K26),K7:K26,1),0)*K7:K26,"##0")&amp;","&amp;M7:M26&amp;","&amp;SUBSTITUTE(SUBSTITUTE(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A26,",",";"),"
 "," ")&amp;CHAR(10),"")</f>
         <v/>
-      </c>
-    </row>
-    <row r="49" spans="9:9" ht="30" hidden="1" customHeight="1">
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" ht="30" hidden="1" customHeight="1">
-      <c r="I50">
-        <v>0</v>
       </c>
     </row>
     <row r="51" spans="9:9" ht="30" hidden="1" customHeight="1">
@@ -2867,6 +2945,21 @@
     </row>
     <row r="66" spans="9:9" ht="30" hidden="1" customHeight="1">
       <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" ht="30" hidden="1" customHeight="1">
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" ht="30" hidden="1" customHeight="1">
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" ht="30" hidden="1" customHeight="1">
+      <c r="I69">
         <v>0</v>
       </c>
     </row>
@@ -2874,271 +2967,285 @@
   <mergeCells count="3">
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="H5:M5"/>
-    <mergeCell ref="I28:L47"/>
+    <mergeCell ref="I29:L49"/>
   </mergeCells>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="3" priority="52">
+    <cfRule type="expression" dxfId="3" priority="54">
       <formula>AND(ISBLANK(D10),ISBLANK(L10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="53">
+    <cfRule type="expression" dxfId="1" priority="55">
       <formula>IF(SUM(H10)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="56" operator="greaterThan">
       <formula>SUM(H10)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="57" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J10),I10,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="3" priority="56">
+    <cfRule type="expression" dxfId="3" priority="58">
       <formula>AND(ISBLANK(D11),ISBLANK(L11))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="57">
+    <cfRule type="expression" dxfId="1" priority="59">
       <formula>IF(SUM(H11)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="60" operator="greaterThan">
       <formula>SUM(H11)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="61" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J11),I11,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="3" priority="60">
+    <cfRule type="expression" dxfId="3" priority="62">
       <formula>AND(ISBLANK(D12),ISBLANK(L12))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="61">
+    <cfRule type="expression" dxfId="1" priority="63">
       <formula>IF(SUM(H12)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="64" operator="greaterThan">
       <formula>SUM(H12)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="65" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J12),I12,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="3" priority="64">
+    <cfRule type="expression" dxfId="3" priority="66">
       <formula>AND(ISBLANK(D13),ISBLANK(L13))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="65">
+    <cfRule type="expression" dxfId="1" priority="67">
       <formula>IF(SUM(H13)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="68" operator="greaterThan">
       <formula>SUM(H13)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="69" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J13),I13,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="3" priority="68">
+    <cfRule type="expression" dxfId="3" priority="70">
       <formula>AND(ISBLANK(D14),ISBLANK(L14))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="69">
+    <cfRule type="expression" dxfId="1" priority="71">
       <formula>IF(SUM(H14)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="greaterThan">
       <formula>SUM(H14)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="73" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J14),I14,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="3" priority="72">
+    <cfRule type="expression" dxfId="3" priority="74">
       <formula>AND(ISBLANK(D15),ISBLANK(L15))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="73">
+    <cfRule type="expression" dxfId="1" priority="75">
       <formula>IF(SUM(H15)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="76" operator="greaterThan">
       <formula>SUM(H15)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="77" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J15),I15,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="3" priority="76">
+    <cfRule type="expression" dxfId="3" priority="78">
       <formula>AND(ISBLANK(D16),ISBLANK(L16))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="77">
+    <cfRule type="expression" dxfId="1" priority="79">
       <formula>IF(SUM(H16)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="80" operator="greaterThan">
       <formula>SUM(H16)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="81" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J16),I16,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="3" priority="80">
+    <cfRule type="expression" dxfId="3" priority="82">
       <formula>AND(ISBLANK(D17),ISBLANK(L17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="81">
+    <cfRule type="expression" dxfId="1" priority="83">
       <formula>IF(SUM(H17)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="84" operator="greaterThan">
       <formula>SUM(H17)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="85" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J17),I17,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="3" priority="84">
+    <cfRule type="expression" dxfId="3" priority="86">
       <formula>AND(ISBLANK(D18),ISBLANK(L18))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="85">
+    <cfRule type="expression" dxfId="1" priority="87">
       <formula>IF(SUM(H18)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="88" operator="greaterThan">
       <formula>SUM(H18)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="89" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J18),I18,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="3" priority="88">
+    <cfRule type="expression" dxfId="3" priority="90">
       <formula>AND(ISBLANK(D19),ISBLANK(L19))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="89">
+    <cfRule type="expression" dxfId="1" priority="91">
       <formula>IF(SUM(H19)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="92" operator="greaterThan">
       <formula>SUM(H19)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="93" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J19),I19,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="3" priority="92">
+    <cfRule type="expression" dxfId="3" priority="94">
       <formula>AND(ISBLANK(D20),ISBLANK(L20))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="93">
+    <cfRule type="expression" dxfId="1" priority="95">
       <formula>IF(SUM(H20)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="96" operator="greaterThan">
       <formula>SUM(H20)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="97" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J20),I20,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="3" priority="96">
+    <cfRule type="expression" dxfId="3" priority="98">
       <formula>AND(ISBLANK(D21),ISBLANK(L21))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="97">
+    <cfRule type="expression" dxfId="1" priority="99">
       <formula>IF(SUM(H21)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="100" operator="greaterThan">
       <formula>SUM(H21)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="101" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J21),I21,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="3" priority="100">
+    <cfRule type="expression" dxfId="3" priority="102">
       <formula>AND(ISBLANK(D22),ISBLANK(L22))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="101">
+    <cfRule type="expression" dxfId="1" priority="103">
       <formula>IF(SUM(H22)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="104" operator="greaterThan">
       <formula>SUM(H22)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="105" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J22),I22,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="3" priority="104">
+    <cfRule type="expression" dxfId="3" priority="106">
       <formula>AND(ISBLANK(D23),ISBLANK(L23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="105">
+    <cfRule type="expression" dxfId="1" priority="107">
       <formula>IF(SUM(H23)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="108" operator="greaterThan">
       <formula>SUM(H23)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="109" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J23),I23,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="3" priority="108">
+    <cfRule type="expression" dxfId="3" priority="110">
       <formula>AND(ISBLANK(D24),ISBLANK(L24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="109">
+    <cfRule type="expression" dxfId="1" priority="111">
       <formula>IF(SUM(H24)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="112" operator="greaterThan">
       <formula>SUM(H24)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="113" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J24),I24,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="3" priority="112">
+    <cfRule type="expression" dxfId="3" priority="114">
       <formula>AND(ISBLANK(D25),ISBLANK(L25))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="113">
+    <cfRule type="expression" dxfId="1" priority="115">
       <formula>IF(SUM(H25)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="116" operator="greaterThan">
       <formula>SUM(H25)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="117" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J25),I25,0))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="expression" dxfId="3" priority="118">
+      <formula>AND(ISBLANK(D26),ISBLANK(L26))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="119">
+      <formula>IF(SUM(H26)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="120" operator="greaterThan">
+      <formula>SUM(H26)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="121" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(J26),I26,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="3" priority="40">
+    <cfRule type="expression" dxfId="3" priority="42">
       <formula>AND(ISBLANK(D7),ISBLANK(L7))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="41">
+    <cfRule type="expression" dxfId="1" priority="43">
       <formula>IF(SUM(H7)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="44" operator="greaterThan">
       <formula>SUM(H7)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="45" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J7),I7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="3" priority="44">
+    <cfRule type="expression" dxfId="3" priority="46">
       <formula>AND(ISBLANK(D8),ISBLANK(L8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="45">
+    <cfRule type="expression" dxfId="1" priority="47">
       <formula>IF(SUM(H8)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="greaterThan">
       <formula>SUM(H8)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="49" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J8),I8,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="3" priority="48">
+    <cfRule type="expression" dxfId="3" priority="50">
       <formula>AND(ISBLANK(D9),ISBLANK(L9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="1" priority="51">
       <formula>IF(SUM(H9)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="greaterThan">
       <formula>SUM(H9)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="53" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(J9),I9,0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3188,7 +3295,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThan">
       <formula>E19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3222,6 +3329,11 @@
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="0" priority="40" operator="lessThan">
+      <formula>E26</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>E7</formula>
@@ -3278,14 +3390,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="2" priority="24">
-      <formula>AND(I18&gt;0,MOD(I18,K18)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="25">
+    <cfRule type="expression" dxfId="1" priority="24">
       <formula>AND(NOT(ISBLANK(I18)),OR(H18="NonStk",I18&gt;H18))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="2" priority="26">
+      <formula>AND(I19&gt;0,MOD(I19,K19)&lt;&gt;0)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(NOT(ISBLANK(I19)),OR(H19="NonStk",I19&gt;H19))</formula>
     </cfRule>
@@ -3318,6 +3430,11 @@
   <conditionalFormatting sqref="I25">
     <cfRule type="expression" dxfId="1" priority="39">
       <formula>AND(NOT(ISBLANK(I25)),OR(H25="NonStk",I25&gt;H25))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="1" priority="41">
+      <formula>AND(NOT(ISBLANK(I26)),OR(H26="NonStk",I26&gt;H26))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
@@ -3349,9 +3466,9 @@
     <hyperlink ref="M12" r:id="rId11"/>
     <hyperlink ref="D13" r:id="rId12"/>
     <hyperlink ref="M13" r:id="rId13"/>
-    <hyperlink ref="M14" r:id="rId14"/>
-    <hyperlink ref="M15" r:id="rId15"/>
-    <hyperlink ref="D16" r:id="rId16"/>
+    <hyperlink ref="D14" r:id="rId14"/>
+    <hyperlink ref="M14" r:id="rId15"/>
+    <hyperlink ref="M15" r:id="rId16"/>
     <hyperlink ref="M16" r:id="rId17"/>
     <hyperlink ref="D17" r:id="rId18"/>
     <hyperlink ref="M17" r:id="rId19"/>
@@ -3371,9 +3488,11 @@
     <hyperlink ref="M24" r:id="rId33"/>
     <hyperlink ref="D25" r:id="rId34"/>
     <hyperlink ref="M25" r:id="rId35"/>
-    <hyperlink ref="H27" r:id="rId36"/>
+    <hyperlink ref="D26" r:id="rId36"/>
+    <hyperlink ref="M26" r:id="rId37"/>
+    <hyperlink ref="H28" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId37"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>